<commit_message>
[Documentation] Update function points
</commit_message>
<xml_diff>
--- a/Documentation/FunctionPoints/FunctionPoints.xlsx
+++ b/Documentation/FunctionPoints/FunctionPoints.xlsx
@@ -5,14 +5,14 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\D067867\Documents\WGPlaner\FunctionPoints\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\D067867\Documents\WGPlaner\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12900"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,78 +24,108 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="31">
   <si>
-    <t>Use Case</t>
+    <t>External Inputs (EI)</t>
+  </si>
+  <si>
+    <t>External Outputs (EO)</t>
+  </si>
+  <si>
+    <t>ShoppingList</t>
+  </si>
+  <si>
+    <t>External Queries (EQ)</t>
+  </si>
+  <si>
+    <t>Internal Logical Files (ILF)</t>
+  </si>
+  <si>
+    <t>External Interface Files (EIF)</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>Complexity</t>
+  </si>
+  <si>
+    <t>RET</t>
+  </si>
+  <si>
+    <t>FTR</t>
+  </si>
+  <si>
+    <t>DET</t>
   </si>
   <si>
     <t>Function Points</t>
   </si>
   <si>
-    <t>New Use Cases</t>
+    <t>Display Details</t>
   </si>
   <si>
-    <t>x: time</t>
-  </si>
-  <si>
-    <t>y: function points</t>
-  </si>
-  <si>
-    <t>AddItem</t>
-  </si>
-  <si>
-    <t>BuyItem</t>
-  </si>
-  <si>
-    <t>InviteMember</t>
-  </si>
-  <si>
-    <t>ProfileSettings</t>
+    <t>Add Item</t>
   </si>
   <si>
     <t>Registration</t>
   </si>
   <si>
-    <t>ShoppingList</t>
+    <t>Profile Settings</t>
   </si>
   <si>
-    <t>Time spent (minutes)</t>
+    <t>Invite new group member</t>
   </si>
   <si>
-    <t>ListBoughtItems</t>
+    <t>Buy Item</t>
   </si>
   <si>
-    <t>ListFixedCosts</t>
+    <t>average</t>
   </si>
   <si>
-    <t>ListReceivedBills</t>
+    <t>External Inquiries (EIQ)</t>
   </si>
   <si>
-    <t>Time Estimation (minutes)</t>
+    <t>complex</t>
+  </si>
+  <si>
+    <t>simple</t>
+  </si>
+  <si>
+    <t>List bought items</t>
+  </si>
+  <si>
+    <t>List received bills</t>
+  </si>
+  <si>
+    <t>List sent bills</t>
+  </si>
+  <si>
+    <t>UseCase</t>
+  </si>
+  <si>
+    <t>Shopping List</t>
+  </si>
+  <si>
+    <t>Time Spent (min)</t>
+  </si>
+  <si>
+    <t>Time Spent / Function Points</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>(Time Spent) = 23.38934231 * (Function Points) + 0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -110,7 +140,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -122,29 +152,7 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
+      <bottom style="double">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -153,54 +161,182 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="56">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -226,8 +362,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="1"/>
-      <tableStyleElement type="headerRow" dxfId="0"/>
+      <tableStyleElement type="wholeTable" dxfId="55"/>
+      <tableStyleElement type="headerRow" dxfId="54"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -255,19 +391,9 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="6.9570401037640672E-2"/>
-          <c:y val="2.6560353854731884E-2"/>
-          <c:w val="0.73206510583847573"/>
-          <c:h val="0.87737205160111953"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -275,10 +401,10 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Implemented Use Cases</c:v>
+            <c:v>Old Use Cases</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="25400" cap="rnd">
               <a:noFill/>
               <a:round/>
             </a:ln>
@@ -286,7 +412,7 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="7"/>
+            <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
@@ -295,7 +421,6 @@
                 <a:solidFill>
                   <a:schemeClr val="accent1"/>
                 </a:solidFill>
-                <a:round/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -311,96 +436,73 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="linear"/>
-            <c:intercept val="0"/>
             <c:dispRSqr val="0"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="0.33286593647507873"/>
-                  <c:y val="-0.12959557321911216"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="de-DE"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Tabelle1!$B$2:$B$7</c:f>
+              <c:f>Sheet1!$B$66:$B$71</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>710</c:v>
+                  <c:v>1030</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>500</c:v>
+                  <c:v>720</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>520</c:v>
+                  <c:v>1625</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>730</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1625</c:v>
+                  <c:v>520</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>790</c:v>
+                  <c:v>620</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabelle1!$C$2:$C$7</c:f>
+              <c:f>Sheet1!$C$66:$C$71</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>29.76</c:v>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18.02</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22.56</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>41.8</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>20</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -408,7 +510,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-E9CC-435A-A74A-24A10578E016}"/>
+              <c16:uniqueId val="{00000000-122F-4CAD-AB73-D8D613CDE0AA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -426,8 +528,8 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="square"/>
-            <c:size val="7"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
@@ -442,36 +544,36 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Tabelle1!$B$10:$B$12</c:f>
+              <c:f>Sheet1!$B$75:$B$77</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>603.92156862745105</c:v>
+                  <c:v>1286.4138268646645</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>590.19607843137248</c:v>
+                  <c:v>631.51224227901719</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>576.47058823529414</c:v>
+                  <c:v>631.51224227901719</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabelle1!$C$10:$C$12</c:f>
+              <c:f>Sheet1!$C$75:$C$77</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>18.48</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18.059999999999999</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17.64</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -479,11 +581,12 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000008-E9CC-435A-A74A-24A10578E016}"/>
+              <c16:uniqueId val="{00000001-122F-4CAD-AB73-D8D613CDE0AA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -491,16 +594,30 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="538422296"/>
-        <c:axId val="538420984"/>
+        <c:axId val="442216224"/>
+        <c:axId val="440070600"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="538422296"/>
+        <c:axId val="442216224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -522,8 +639,13 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="de-DE"/>
-                  <a:t>Time spent</a:t>
+                  <a:t>Time</a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="de-DE" baseline="0"/>
+                  <a:t> Spent (min)</a:t>
+                </a:r>
+                <a:endParaRPr lang="de-DE"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -557,7 +679,7 @@
           </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -593,12 +715,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="538420984"/>
+        <c:crossAx val="440070600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="538420984"/>
+        <c:axId val="440070600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -618,20 +740,6 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:minorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="5000"/>
-                  <a:lumOff val="95000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:minorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -688,7 +796,7 @@
           </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -724,7 +832,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="538422296"/>
+        <c:crossAx val="442216224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -736,47 +844,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.81672378387934674"/>
-          <c:y val="0.44529936999366165"/>
-          <c:w val="0.17464063753688816"/>
-          <c:h val="0.2304167570625795"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -808,7 +875,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1374,23 +1441,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>65890</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>20619</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="8" name="Diagramm 7">
+        <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB0EB762-5DBD-4C58-8ABE-DA8E852475E8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B6DE25D-DA1F-47D6-BB86-8FCB1B7D7A9D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1409,6 +1476,150 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:G7" totalsRowShown="0">
+  <autoFilter ref="A2:G7"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="Display Details"/>
+    <tableColumn id="2" name="Count" dataDxfId="38"/>
+    <tableColumn id="3" name="Complexity" dataDxfId="36"/>
+    <tableColumn id="4" name="RET" dataDxfId="37"/>
+    <tableColumn id="5" name="FTR" dataDxfId="53"/>
+    <tableColumn id="6" name="DET" dataDxfId="52"/>
+    <tableColumn id="7" name="Function Points" dataDxfId="51"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A9:G14" totalsRowShown="0">
+  <autoFilter ref="A9:G14"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="Display Details"/>
+    <tableColumn id="2" name="Count" dataDxfId="35"/>
+    <tableColumn id="3" name="Complexity" dataDxfId="33"/>
+    <tableColumn id="4" name="RET" dataDxfId="34"/>
+    <tableColumn id="5" name="FTR" dataDxfId="50"/>
+    <tableColumn id="6" name="DET" dataDxfId="49"/>
+    <tableColumn id="7" name="Function Points" dataDxfId="48"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A16:G21" totalsRowShown="0">
+  <autoFilter ref="A16:G21"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="Display Details"/>
+    <tableColumn id="2" name="Count" dataDxfId="32"/>
+    <tableColumn id="3" name="Complexity" dataDxfId="30"/>
+    <tableColumn id="4" name="RET" dataDxfId="31"/>
+    <tableColumn id="5" name="FTR" dataDxfId="47"/>
+    <tableColumn id="6" name="DET" dataDxfId="46"/>
+    <tableColumn id="7" name="Function Points" dataDxfId="45"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table15" displayName="Table15" ref="A23:G28" totalsRowShown="0">
+  <autoFilter ref="A23:G28"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="Display Details"/>
+    <tableColumn id="2" name="Count" dataDxfId="29"/>
+    <tableColumn id="3" name="Complexity" dataDxfId="27"/>
+    <tableColumn id="4" name="RET" dataDxfId="28"/>
+    <tableColumn id="5" name="FTR" dataDxfId="44"/>
+    <tableColumn id="6" name="DET" dataDxfId="43"/>
+    <tableColumn id="7" name="Function Points" dataDxfId="42"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table16" displayName="Table16" ref="A30:G35" totalsRowShown="0">
+  <autoFilter ref="A30:G35"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="Display Details"/>
+    <tableColumn id="2" name="Count" dataDxfId="26"/>
+    <tableColumn id="3" name="Complexity" dataDxfId="24"/>
+    <tableColumn id="4" name="RET" dataDxfId="25"/>
+    <tableColumn id="5" name="FTR" dataDxfId="41"/>
+    <tableColumn id="6" name="DET" dataDxfId="40"/>
+    <tableColumn id="7" name="Function Points" dataDxfId="39"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table167" displayName="Table167" ref="A37:G42" totalsRowShown="0">
+  <autoFilter ref="A37:G42"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="Display Details"/>
+    <tableColumn id="2" name="Count" dataDxfId="23"/>
+    <tableColumn id="3" name="Complexity" dataDxfId="22"/>
+    <tableColumn id="4" name="RET" dataDxfId="21"/>
+    <tableColumn id="5" name="FTR" dataDxfId="20"/>
+    <tableColumn id="6" name="DET" dataDxfId="19"/>
+    <tableColumn id="7" name="Function Points" dataDxfId="18"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table1678" displayName="Table1678" ref="A44:G49" totalsRowShown="0">
+  <autoFilter ref="A44:G49"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="Display Details"/>
+    <tableColumn id="2" name="Count" dataDxfId="17"/>
+    <tableColumn id="3" name="Complexity" dataDxfId="16"/>
+    <tableColumn id="4" name="RET" dataDxfId="15"/>
+    <tableColumn id="5" name="FTR" dataDxfId="14"/>
+    <tableColumn id="6" name="DET" dataDxfId="13"/>
+    <tableColumn id="7" name="Function Points" dataDxfId="12"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table16789" displayName="Table16789" ref="A51:G56" totalsRowShown="0">
+  <autoFilter ref="A51:G56"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="Display Details"/>
+    <tableColumn id="2" name="Count" dataDxfId="11"/>
+    <tableColumn id="3" name="Complexity" dataDxfId="10"/>
+    <tableColumn id="4" name="RET" dataDxfId="9"/>
+    <tableColumn id="5" name="FTR" dataDxfId="8"/>
+    <tableColumn id="6" name="DET" dataDxfId="7"/>
+    <tableColumn id="7" name="Function Points" dataDxfId="6"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table1678910" displayName="Table1678910" ref="A58:G63" totalsRowShown="0">
+  <autoFilter ref="A58:G63"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="Display Details"/>
+    <tableColumn id="2" name="Count" dataDxfId="4"/>
+    <tableColumn id="3" name="Complexity" dataDxfId="3"/>
+    <tableColumn id="4" name="RET" dataDxfId="2"/>
+    <tableColumn id="5" name="FTR" dataDxfId="1"/>
+    <tableColumn id="6" name="DET" dataDxfId="0"/>
+    <tableColumn id="7" name="Function Points" dataDxfId="5"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1708,225 +1919,1339 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:G82"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M33" sqref="M33"/>
+    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="D84" sqref="D84"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="27.5703125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" style="4" customWidth="1"/>
-    <col min="4" max="16384" width="11.42578125" style="4"/>
+    <col min="1" max="1" width="36.42578125" customWidth="1"/>
+    <col min="2" max="7" width="36.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B3" s="1">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1">
+        <v>2</v>
+      </c>
+      <c r="F3" s="1">
+        <v>19</v>
+      </c>
+      <c r="G3" s="1">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1">
+        <v>2</v>
+      </c>
+      <c r="F4" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="1">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="1">
+        <v>2</v>
+      </c>
+      <c r="E5" s="1">
+        <v>3</v>
+      </c>
+      <c r="F5" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="1">
+        <v>3</v>
+      </c>
+      <c r="E7" s="1">
+        <v>3</v>
+      </c>
+      <c r="F7" s="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="1">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="1">
+        <v>6</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="1">
+        <v>2</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1</v>
+      </c>
+      <c r="F10" s="1">
         <v>5</v>
       </c>
-      <c r="B2" s="5">
-        <v>710</v>
-      </c>
-      <c r="C2" s="5">
-        <v>29.76</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="G10" s="1">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="1">
+        <v>5</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1">
+        <v>1</v>
+      </c>
+      <c r="F11" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1">
+        <v>1</v>
+      </c>
+      <c r="F13" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1</v>
+      </c>
+      <c r="F14" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" s="1">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="5">
-        <v>500</v>
-      </c>
-      <c r="C3" s="5">
-        <v>18.02</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="5">
+      <c r="D16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="1">
+        <v>10</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1</v>
+      </c>
+      <c r="E17" s="1">
+        <v>1</v>
+      </c>
+      <c r="F17" s="1">
+        <v>3</v>
+      </c>
+      <c r="G17" s="1">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="1">
+        <v>3</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1</v>
+      </c>
+      <c r="F18" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="1">
+        <v>3</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="1">
+        <v>1</v>
+      </c>
+      <c r="E19" s="1">
+        <v>1</v>
+      </c>
+      <c r="F19" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="1">
+        <v>1</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" s="1">
+        <v>1</v>
+      </c>
+      <c r="E21" s="1">
+        <v>1</v>
+      </c>
+      <c r="F21" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>15</v>
+      </c>
+      <c r="G22" s="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="1">
+        <v>3</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" s="1">
+        <v>1</v>
+      </c>
+      <c r="E24" s="1">
+        <v>1</v>
+      </c>
+      <c r="F24" s="1">
+        <v>3</v>
+      </c>
+      <c r="G24" s="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="1">
+        <v>2</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" s="1">
+        <v>2</v>
+      </c>
+      <c r="E25" s="1">
+        <v>2</v>
+      </c>
+      <c r="F25" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" s="1">
+        <v>1</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D26" s="1">
+        <v>1</v>
+      </c>
+      <c r="E26" s="1">
+        <v>1</v>
+      </c>
+      <c r="F26" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="1">
+        <v>0</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" s="1">
+        <v>1</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D28" s="1">
+        <v>1</v>
+      </c>
+      <c r="E28" s="1">
+        <v>1</v>
+      </c>
+      <c r="F28" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>16</v>
+      </c>
+      <c r="G29" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" s="1">
+        <v>3</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D31" s="1">
+        <v>1</v>
+      </c>
+      <c r="E31" s="1">
+        <v>1</v>
+      </c>
+      <c r="F31" s="1">
+        <v>1</v>
+      </c>
+      <c r="G31" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" s="1">
+        <v>1</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D32" s="1">
+        <v>1</v>
+      </c>
+      <c r="E32" s="1">
+        <v>1</v>
+      </c>
+      <c r="F32" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33" s="1">
+        <v>1</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D33" s="1">
+        <v>1</v>
+      </c>
+      <c r="E33" s="1">
+        <v>1</v>
+      </c>
+      <c r="F33" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" s="1">
+        <v>0</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35" s="1">
+        <v>1</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D35" s="1">
+        <v>1</v>
+      </c>
+      <c r="E35" s="1">
+        <v>1</v>
+      </c>
+      <c r="F35" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>17</v>
+      </c>
+      <c r="G36" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>12</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>0</v>
+      </c>
+      <c r="B38" s="1">
+        <v>2</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D38" s="1">
+        <v>1</v>
+      </c>
+      <c r="E38" s="1">
+        <v>1</v>
+      </c>
+      <c r="F38" s="1">
+        <v>1</v>
+      </c>
+      <c r="G38" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>1</v>
+      </c>
+      <c r="B39" s="1">
+        <v>1</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D39" s="1">
+        <v>1</v>
+      </c>
+      <c r="E39" s="1">
+        <v>1</v>
+      </c>
+      <c r="F39" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>19</v>
+      </c>
+      <c r="B40" s="1">
+        <v>1</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D40" s="1">
+        <v>1</v>
+      </c>
+      <c r="E40" s="1">
+        <v>1</v>
+      </c>
+      <c r="F40" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>4</v>
+      </c>
+      <c r="B41" s="1">
+        <v>0</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>5</v>
+      </c>
+      <c r="B42" s="1">
+        <v>1</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D42" s="1">
+        <v>1</v>
+      </c>
+      <c r="E42" s="1">
+        <v>1</v>
+      </c>
+      <c r="F42" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>22</v>
+      </c>
+      <c r="G43" s="1">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>12</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>0</v>
+      </c>
+      <c r="B45" s="1">
+        <v>5</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D45" s="1">
+        <v>4</v>
+      </c>
+      <c r="E45" s="1">
+        <v>4</v>
+      </c>
+      <c r="F45" s="1">
+        <v>19</v>
+      </c>
+      <c r="G45" s="1">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>1</v>
+      </c>
+      <c r="B46" s="1">
+        <v>2</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D46" s="1">
+        <v>2</v>
+      </c>
+      <c r="E46" s="1">
+        <v>2</v>
+      </c>
+      <c r="F46" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>19</v>
+      </c>
+      <c r="B47" s="1">
+        <v>1</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D47" s="1">
+        <v>2</v>
+      </c>
+      <c r="E47" s="1">
+        <v>1</v>
+      </c>
+      <c r="F47" s="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>4</v>
+      </c>
+      <c r="B48" s="1">
+        <v>0</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>5</v>
+      </c>
+      <c r="B49" s="1">
+        <v>2</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D49" s="1">
+        <v>2</v>
+      </c>
+      <c r="E49" s="1">
+        <v>1</v>
+      </c>
+      <c r="F49" s="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>23</v>
+      </c>
+      <c r="G50" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>12</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>0</v>
+      </c>
+      <c r="B52" s="1">
+        <v>1</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D52" s="1">
+        <v>1</v>
+      </c>
+      <c r="E52" s="1">
+        <v>1</v>
+      </c>
+      <c r="F52" s="1">
+        <v>1</v>
+      </c>
+      <c r="G52" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>1</v>
+      </c>
+      <c r="B53" s="1">
+        <v>1</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D53" s="1">
+        <v>2</v>
+      </c>
+      <c r="E53" s="1">
+        <v>1</v>
+      </c>
+      <c r="F53" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>19</v>
+      </c>
+      <c r="B54" s="1">
+        <v>2</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D54" s="1">
+        <v>3</v>
+      </c>
+      <c r="E54" s="1">
+        <v>1</v>
+      </c>
+      <c r="F54" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>4</v>
+      </c>
+      <c r="B55" s="1">
+        <v>0</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>5</v>
+      </c>
+      <c r="B56" s="1">
+        <v>2</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D56" s="1">
+        <v>3</v>
+      </c>
+      <c r="E56" s="1">
+        <v>1</v>
+      </c>
+      <c r="F56" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>24</v>
+      </c>
+      <c r="G57" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>12</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>0</v>
+      </c>
+      <c r="B59" s="1">
+        <v>1</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D59" s="1">
+        <v>1</v>
+      </c>
+      <c r="E59" s="1">
+        <v>1</v>
+      </c>
+      <c r="F59" s="1">
+        <v>1</v>
+      </c>
+      <c r="G59" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>1</v>
+      </c>
+      <c r="B60" s="1">
+        <v>1</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D60" s="1">
+        <v>2</v>
+      </c>
+      <c r="E60" s="1">
+        <v>1</v>
+      </c>
+      <c r="F60" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>19</v>
+      </c>
+      <c r="B61" s="1">
+        <v>2</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D61" s="1">
+        <v>3</v>
+      </c>
+      <c r="E61" s="1">
+        <v>1</v>
+      </c>
+      <c r="F61" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>4</v>
+      </c>
+      <c r="B62" s="1">
+        <v>0</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>5</v>
+      </c>
+      <c r="B63" s="1">
+        <v>2</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D63" s="1">
+        <v>3</v>
+      </c>
+      <c r="E63" s="1">
+        <v>1</v>
+      </c>
+      <c r="F63" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>25</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>26</v>
+      </c>
+      <c r="B66" s="1">
+        <v>1030</v>
+      </c>
+      <c r="C66" s="1">
+        <v>92</v>
+      </c>
+      <c r="D66" s="1">
+        <f>B66/C66</f>
+        <v>11.195652173913043</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>13</v>
+      </c>
+      <c r="B67" s="1">
+        <v>720</v>
+      </c>
+      <c r="C67" s="1">
+        <v>54</v>
+      </c>
+      <c r="D67" s="1">
+        <f t="shared" ref="D67:D71" si="0">B67/C67</f>
+        <v>13.333333333333334</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>14</v>
+      </c>
+      <c r="B68" s="1">
+        <v>1625</v>
+      </c>
+      <c r="C68" s="1">
+        <v>62</v>
+      </c>
+      <c r="D68" s="1">
+        <f t="shared" si="0"/>
+        <v>26.20967741935484</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>15</v>
+      </c>
+      <c r="B69" s="1">
+        <v>730</v>
+      </c>
+      <c r="C69" s="1">
+        <v>26</v>
+      </c>
+      <c r="D69" s="1">
+        <f t="shared" si="0"/>
+        <v>28.076923076923077</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>16</v>
+      </c>
+      <c r="B70" s="1">
         <v>520</v>
       </c>
-      <c r="C4" s="5">
-        <v>22.56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="5">
-        <v>730</v>
-      </c>
-      <c r="C5" s="5">
+      <c r="C70" s="1">
+        <v>18</v>
+      </c>
+      <c r="D70" s="1">
+        <f t="shared" si="0"/>
+        <v>28.888888888888889</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B71" s="3">
+        <v>620</v>
+      </c>
+      <c r="C71" s="3">
+        <v>19</v>
+      </c>
+      <c r="D71" s="3">
+        <f t="shared" si="0"/>
+        <v>32.631578947368418</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C72" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D72" s="1">
+        <f>SUM(D66:D71)/6</f>
+        <v>23.389342306630265</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>25</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>22</v>
+      </c>
+      <c r="B75" s="1">
+        <f>C75*$D$72</f>
+        <v>1286.4138268646645</v>
+      </c>
+      <c r="C75" s="1">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>23</v>
+      </c>
+      <c r="B76" s="1">
+        <f t="shared" ref="B76:B77" si="1">C76*$D$72</f>
+        <v>631.51224227901719</v>
+      </c>
+      <c r="C76" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>24</v>
+      </c>
+      <c r="B77" s="1">
+        <f t="shared" si="1"/>
+        <v>631.51224227901719</v>
+      </c>
+      <c r="C77" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="82" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E82" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="5">
-        <v>1625</v>
-      </c>
-      <c r="C6" s="5">
-        <v>41.8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="5">
-        <v>790</v>
-      </c>
-      <c r="C7" s="5">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
-      <c r="C8" s="6"/>
-    </row>
-    <row r="9" spans="1:3" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="14">
-        <f>C10/0.0306</f>
-        <v>603.92156862745105</v>
-      </c>
-      <c r="C10" s="5">
-        <v>18.48</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="14">
-        <f t="shared" ref="B11:B12" si="0">C11/0.0306</f>
-        <v>590.19607843137248</v>
-      </c>
-      <c r="C11" s="5">
-        <v>18.059999999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="14">
-        <f t="shared" si="0"/>
-        <v>576.47058823529414</v>
-      </c>
-      <c r="C12" s="5">
-        <v>17.64</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
-      <c r="C13" s="6"/>
-    </row>
-    <row r="14" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
-      <c r="C14" s="6"/>
-    </row>
-    <row r="15" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" s="6"/>
-    </row>
-    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" s="6"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C17" s="6"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="9"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-    </row>
-    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="9"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="9"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="9"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="9"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="9"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="9"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="9"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="9"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="9"/>
-      <c r="B24" s="11"/>
-      <c r="C24" s="9"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="9"/>
-      <c r="B25" s="9"/>
-      <c r="C25" s="9"/>
-    </row>
-    <row r="26" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="9"/>
-      <c r="B26" s="12"/>
-      <c r="C26" s="9"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="9"/>
-      <c r="B27" s="16"/>
-      <c r="C27" s="9"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B28" s="17"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B29" s="17"/>
-    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="9">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId8"/>
+    <tablePart r:id="rId9"/>
+    <tablePart r:id="rId10"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[UC] Update function points
</commit_message>
<xml_diff>
--- a/Documentation/FunctionPoints/FunctionPoints.xlsx
+++ b/Documentation/FunctionPoints/FunctionPoints.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\D067867\Documents\WGPlaner\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\D067866\AndroidStudioProjects\WGPlaner\Documentation\FunctionPoints\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="30">
   <si>
     <t>External Inputs (EI)</t>
   </si>
@@ -113,10 +113,7 @@
     <t>Time Spent / Function Points</t>
   </si>
   <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>(Time Spent) = 23.38934231 * (Function Points) + 0</t>
+    <t>(Time Spent) = (Function Points) / 0.0508</t>
   </si>
 </sst>
 </file>
@@ -436,22 +433,45 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="linear"/>
+            <c:intercept val="0"/>
             <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.5225838284574741E-2"/>
+                  <c:y val="-1.8666824938339995E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="de-DE"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -549,13 +569,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1286.4138268646645</c:v>
+                  <c:v>1082.6771653543308</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>631.51224227901719</c:v>
+                  <c:v>531.49606299212599</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>631.51224227901719</c:v>
+                  <c:v>531.49606299212599</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -586,7 +606,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -1483,12 +1502,12 @@
   <autoFilter ref="A2:G7"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Display Details"/>
-    <tableColumn id="2" name="Count" dataDxfId="38"/>
-    <tableColumn id="3" name="Complexity" dataDxfId="36"/>
-    <tableColumn id="4" name="RET" dataDxfId="37"/>
-    <tableColumn id="5" name="FTR" dataDxfId="53"/>
-    <tableColumn id="6" name="DET" dataDxfId="52"/>
-    <tableColumn id="7" name="Function Points" dataDxfId="51"/>
+    <tableColumn id="2" name="Count" dataDxfId="53"/>
+    <tableColumn id="3" name="Complexity" dataDxfId="52"/>
+    <tableColumn id="4" name="RET" dataDxfId="51"/>
+    <tableColumn id="5" name="FTR" dataDxfId="50"/>
+    <tableColumn id="6" name="DET" dataDxfId="49"/>
+    <tableColumn id="7" name="Function Points" dataDxfId="48"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1499,12 +1518,12 @@
   <autoFilter ref="A9:G14"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Display Details"/>
-    <tableColumn id="2" name="Count" dataDxfId="35"/>
-    <tableColumn id="3" name="Complexity" dataDxfId="33"/>
-    <tableColumn id="4" name="RET" dataDxfId="34"/>
-    <tableColumn id="5" name="FTR" dataDxfId="50"/>
-    <tableColumn id="6" name="DET" dataDxfId="49"/>
-    <tableColumn id="7" name="Function Points" dataDxfId="48"/>
+    <tableColumn id="2" name="Count" dataDxfId="47"/>
+    <tableColumn id="3" name="Complexity" dataDxfId="46"/>
+    <tableColumn id="4" name="RET" dataDxfId="45"/>
+    <tableColumn id="5" name="FTR" dataDxfId="44"/>
+    <tableColumn id="6" name="DET" dataDxfId="43"/>
+    <tableColumn id="7" name="Function Points" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1515,12 +1534,12 @@
   <autoFilter ref="A16:G21"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Display Details"/>
-    <tableColumn id="2" name="Count" dataDxfId="32"/>
-    <tableColumn id="3" name="Complexity" dataDxfId="30"/>
-    <tableColumn id="4" name="RET" dataDxfId="31"/>
-    <tableColumn id="5" name="FTR" dataDxfId="47"/>
-    <tableColumn id="6" name="DET" dataDxfId="46"/>
-    <tableColumn id="7" name="Function Points" dataDxfId="45"/>
+    <tableColumn id="2" name="Count" dataDxfId="41"/>
+    <tableColumn id="3" name="Complexity" dataDxfId="40"/>
+    <tableColumn id="4" name="RET" dataDxfId="39"/>
+    <tableColumn id="5" name="FTR" dataDxfId="38"/>
+    <tableColumn id="6" name="DET" dataDxfId="37"/>
+    <tableColumn id="7" name="Function Points" dataDxfId="36"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1531,12 +1550,12 @@
   <autoFilter ref="A23:G28"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Display Details"/>
-    <tableColumn id="2" name="Count" dataDxfId="29"/>
-    <tableColumn id="3" name="Complexity" dataDxfId="27"/>
-    <tableColumn id="4" name="RET" dataDxfId="28"/>
-    <tableColumn id="5" name="FTR" dataDxfId="44"/>
-    <tableColumn id="6" name="DET" dataDxfId="43"/>
-    <tableColumn id="7" name="Function Points" dataDxfId="42"/>
+    <tableColumn id="2" name="Count" dataDxfId="35"/>
+    <tableColumn id="3" name="Complexity" dataDxfId="34"/>
+    <tableColumn id="4" name="RET" dataDxfId="33"/>
+    <tableColumn id="5" name="FTR" dataDxfId="32"/>
+    <tableColumn id="6" name="DET" dataDxfId="31"/>
+    <tableColumn id="7" name="Function Points" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1547,12 +1566,12 @@
   <autoFilter ref="A30:G35"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Display Details"/>
-    <tableColumn id="2" name="Count" dataDxfId="26"/>
-    <tableColumn id="3" name="Complexity" dataDxfId="24"/>
-    <tableColumn id="4" name="RET" dataDxfId="25"/>
-    <tableColumn id="5" name="FTR" dataDxfId="41"/>
-    <tableColumn id="6" name="DET" dataDxfId="40"/>
-    <tableColumn id="7" name="Function Points" dataDxfId="39"/>
+    <tableColumn id="2" name="Count" dataDxfId="29"/>
+    <tableColumn id="3" name="Complexity" dataDxfId="28"/>
+    <tableColumn id="4" name="RET" dataDxfId="27"/>
+    <tableColumn id="5" name="FTR" dataDxfId="26"/>
+    <tableColumn id="6" name="DET" dataDxfId="25"/>
+    <tableColumn id="7" name="Function Points" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1611,12 +1630,12 @@
   <autoFilter ref="A58:G63"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Display Details"/>
-    <tableColumn id="2" name="Count" dataDxfId="4"/>
-    <tableColumn id="3" name="Complexity" dataDxfId="3"/>
-    <tableColumn id="4" name="RET" dataDxfId="2"/>
-    <tableColumn id="5" name="FTR" dataDxfId="1"/>
-    <tableColumn id="6" name="DET" dataDxfId="0"/>
-    <tableColumn id="7" name="Function Points" dataDxfId="5"/>
+    <tableColumn id="2" name="Count" dataDxfId="5"/>
+    <tableColumn id="3" name="Complexity" dataDxfId="4"/>
+    <tableColumn id="4" name="RET" dataDxfId="3"/>
+    <tableColumn id="5" name="FTR" dataDxfId="2"/>
+    <tableColumn id="6" name="DET" dataDxfId="1"/>
+    <tableColumn id="7" name="Function Points" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1919,10 +1938,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G82"/>
+  <dimension ref="A1:G84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="D84" sqref="D84"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="C80" sqref="C80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3178,15 +3197,7 @@
         <v>32.631578947368418</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C72" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D72" s="1">
-        <f>SUM(D66:D71)/6</f>
-        <v>23.389342306630265</v>
-      </c>
-    </row>
+    <row r="72" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>25</v>
@@ -3203,8 +3214,8 @@
         <v>22</v>
       </c>
       <c r="B75" s="1">
-        <f>C75*$D$72</f>
-        <v>1286.4138268646645</v>
+        <f>C75/$D$84</f>
+        <v>1082.6771653543308</v>
       </c>
       <c r="C75" s="1">
         <v>55</v>
@@ -3215,8 +3226,8 @@
         <v>23</v>
       </c>
       <c r="B76" s="1">
-        <f t="shared" ref="B76:B77" si="1">C76*$D$72</f>
-        <v>631.51224227901719</v>
+        <f t="shared" ref="B76:B77" si="1">C76/$D$84</f>
+        <v>531.49606299212599</v>
       </c>
       <c r="C76" s="1">
         <v>27</v>
@@ -3228,15 +3239,20 @@
       </c>
       <c r="B77" s="1">
         <f t="shared" si="1"/>
-        <v>631.51224227901719</v>
+        <v>531.49606299212599</v>
       </c>
       <c r="C77" s="1">
         <v>27</v>
       </c>
     </row>
-    <row r="82" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E82" s="1" t="s">
-        <v>30</v>
+    <row r="82" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D82" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="84" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D84" s="1">
+        <v>5.0799999999999998E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>